<commit_message>
added some checks and consistency to the Excel file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -2,27 +2,34 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -46,11 +53,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,10 +421,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C11"/>
+  <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -441,88 +449,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>25/01/2024</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>25/01/2024</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="4"/>
+    <row r="5"/>
     <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>25/01/2024</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>25/01/2024</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>25/01/2024</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>25/01/2024</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>25/01/2024</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>25/01/2024</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>9</v>
-      </c>
+      <c r="E6" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
cleaned the code a bit, now the Excel file adds up the counter even if it's the same day
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -424,10 +424,13 @@
   <dimension ref="B1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12.42578125" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1"/>
     <row r="2">
@@ -448,8 +451,10 @@
           <t>25/01/2024</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>20</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>21.0</t>
+        </is>
       </c>
     </row>
     <row r="4"/>

</xml_diff>